<commit_message>
POCs et Upload feature
</commit_message>
<xml_diff>
--- a/src/middleware/input_short.xlsx
+++ b/src/middleware/input_short.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>https://www.labanquepostale.fr/</t>
   </si>
@@ -78,6 +78,15 @@
   </si>
   <si>
     <t>Parcours</t>
+  </si>
+  <si>
+    <t>https://logs.xiti.com/hit.xiti?s=388889&amp;s2=1&amp;p=particuliers::accueil_PARTICULIERS&amp;hl=23x52x18&amp;xtor=sec-322800100-goo-[retraite_generique%20%2B%20marque_bmm]-[103507913820]-s-[%2Bperp%20%2Bla%20%2Bposte]&amp;roinbh=392&amp;ac=&amp;an=&amp;lng=en-US&amp;idp=2352183188828&amp;jv=0&amp;re=625x803&amp;vtag=44007&amp;hl=23x52x18&amp;r=1440x900x24x24&amp;ref=</t>
+  </si>
+  <si>
+    <t>https://logs.xiti.com/hit.xiti?s=388889&amp;s2=21&amp;p=Outils::aide::cookies&amp;hl=23x52x56&amp;xtor=sec-322800100-goo-[retraite_generique%20%2B%20marque_bmm]-[103507913820]-s-[%2Bperp%20%2Bla%20%2Bposte]&amp;roinbh=392&amp;ac=&amp;an=&amp;lng=en-US&amp;idp=2352563949647&amp;jv=0&amp;re=625x803&amp;vtag=44007&amp;hl=23x52x56&amp;r=1440x900x24x24&amp;ref=</t>
+  </si>
+  <si>
+    <t>https://logs.xiti.com/hit.xiti?s=388889&amp;s2=21&amp;p=projets&amp;hl=23x53x12&amp;xtor=sec-322800100-goo-[retraite_generique%20%2B%20marque_bmm]-[103507913820]-s-[%2Bperp%20%2Bla%20%2Bposte]&amp;roinbh=392&amp;ac=&amp;an=&amp;lng=en-US&amp;idp=2353124427578&amp;jv=0&amp;re=625x803&amp;vtag=44007&amp;hl=23x53x12&amp;r=1440x900x24x24&amp;ref=</t>
   </si>
 </sst>
 </file>
@@ -429,7 +438,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -503,6 +512,9 @@
       <c r="B4" t="s">
         <v>0</v>
       </c>
+      <c r="C4" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -511,6 +523,9 @@
       <c r="B5" t="s">
         <v>1</v>
       </c>
+      <c r="C5" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -518,6 +533,9 @@
       </c>
       <c r="B6" t="s">
         <v>2</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>